<commit_message>
Auto commit - 10031357
</commit_message>
<xml_diff>
--- a/IM/202510_Service_Count_Report.xlsx
+++ b/IM/202510_Service_Count_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AA$68</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AA$79</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="241">
   <si>
     <t>服務次數統計表        篩選月份：202510</t>
   </si>
@@ -152,16 +152,16 @@
     <t>住商石牌</t>
   </si>
   <si>
+    <t>抄表</t>
+  </si>
+  <si>
+    <t>PM抄表</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
     <t>服務</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>PM抄表</t>
-  </si>
-  <si>
-    <t>抄表</t>
   </si>
   <si>
     <t>10:30:00</t>
@@ -403,6 +403,24 @@
     <t>湯家瑋</t>
   </si>
   <si>
+    <t>2025-10-03</t>
+  </si>
+  <si>
+    <t>T251000051</t>
+  </si>
+  <si>
+    <t>eS-2510AC 彩色複合機</t>
+  </si>
+  <si>
+    <t xml:space="preserve">沛盈實業有限公司 </t>
+  </si>
+  <si>
+    <t>新北市新莊區中正路665號9樓</t>
+  </si>
+  <si>
+    <t>pm</t>
+  </si>
+  <si>
     <t>08:30:00</t>
   </si>
   <si>
@@ -412,9 +430,6 @@
     <t>T251000056</t>
   </si>
   <si>
-    <t>eS-2510AC 彩色複合機</t>
-  </si>
-  <si>
     <t xml:space="preserve">奧創資訊股份有限公司 </t>
   </si>
   <si>
@@ -442,6 +457,18 @@
     <t>行政組</t>
   </si>
   <si>
+    <t>T252000102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">仲誠不動產經紀有限公司 </t>
+  </si>
+  <si>
+    <t>新北市三重區重新路3段110號</t>
+  </si>
+  <si>
+    <t>三重</t>
+  </si>
+  <si>
     <t>13:30:00</t>
   </si>
   <si>
@@ -457,9 +484,6 @@
     <t>林口文化2F放款部</t>
   </si>
   <si>
-    <t>pm</t>
-  </si>
-  <si>
     <t>測試正常</t>
   </si>
   <si>
@@ -475,9 +499,6 @@
     <t>新北市三重區德厚街76號7樓</t>
   </si>
   <si>
-    <t>三重</t>
-  </si>
-  <si>
     <t>11:45:00</t>
   </si>
   <si>
@@ -514,6 +535,15 @@
     <t>4F</t>
   </si>
   <si>
+    <t>T302800012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">捷旺宅不動產經紀有限公司 </t>
+  </si>
+  <si>
+    <t>新北市三重區捷運路32號</t>
+  </si>
+  <si>
     <t>T302800057</t>
   </si>
   <si>
@@ -652,6 +682,27 @@
     <t>五股檢品</t>
   </si>
   <si>
+    <t>T351800123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">喬治費歇爾機械股份有限公司 </t>
+  </si>
+  <si>
+    <t>新北市三重區興德路94號</t>
+  </si>
+  <si>
+    <t>T352500148</t>
+  </si>
+  <si>
+    <t>eS-3525AC 彩色複合機</t>
+  </si>
+  <si>
+    <t xml:space="preserve">宏偉營造股份有限公司 </t>
+  </si>
+  <si>
+    <t>新北市三重區光復路1段61巷26號2樓</t>
+  </si>
+  <si>
     <t>T452800047</t>
   </si>
   <si>
@@ -677,6 +728,30 @@
   </si>
   <si>
     <t>12:30:00</t>
+  </si>
+  <si>
+    <t>狄澤洋</t>
+  </si>
+  <si>
+    <t>TX30000054</t>
+  </si>
+  <si>
+    <t>TCx300 POS 終端系統</t>
+  </si>
+  <si>
+    <t>POS商品</t>
+  </si>
+  <si>
+    <t xml:space="preserve">台灣泛亞零售管理顧問股份有限公司 </t>
+  </si>
+  <si>
+    <t>台北市萬華區西寧南路123號</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>更換DS4608usb線材</t>
   </si>
   <si>
     <t>合計</t>
@@ -1093,10 +1168,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AB68"/>
+  <dimension ref="A1:AB79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A68" sqref="A68"/>
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1254,7 +1329,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="7">
-        <v>2025100146</v>
+        <v>2025100147</v>
       </c>
       <c r="C3" s="7">
         <v>1</v>
@@ -1302,9 +1377,7 @@
       <c r="R3" s="7">
         <v>105</v>
       </c>
-      <c r="S3" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="S3" s="7"/>
       <c r="T3" s="7"/>
       <c r="U3" s="7"/>
       <c r="V3" s="7"/>
@@ -1312,10 +1385,10 @@
       <c r="X3" s="7"/>
       <c r="Y3" s="7"/>
       <c r="Z3" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AA3" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB3" s="7">
         <v>1</v>
@@ -1326,7 +1399,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3">
-        <v>2025100147</v>
+        <v>2025100146</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
@@ -1374,7 +1447,9 @@
       <c r="R4" s="3">
         <v>105</v>
       </c>
-      <c r="S4" s="3"/>
+      <c r="S4" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="T4" s="3"/>
       <c r="U4" s="3"/>
       <c r="V4" s="3"/>
@@ -1382,10 +1457,10 @@
       <c r="X4" s="3"/>
       <c r="Y4" s="3"/>
       <c r="Z4" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB4" s="3"/>
     </row>
@@ -1394,7 +1469,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="7">
-        <v>2025100023</v>
+        <v>2025100022</v>
       </c>
       <c r="C5" s="7">
         <v>1</v>
@@ -1442,7 +1517,9 @@
       <c r="R5" s="7">
         <v>159</v>
       </c>
-      <c r="S5" s="7"/>
+      <c r="S5" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="T5" s="7"/>
       <c r="U5" s="7"/>
       <c r="V5" s="7"/>
@@ -1450,10 +1527,10 @@
       <c r="X5" s="7"/>
       <c r="Y5" s="7"/>
       <c r="Z5" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AA5" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB5" s="7">
         <v>1</v>
@@ -1464,7 +1541,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3">
-        <v>2025100022</v>
+        <v>2025100023</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
@@ -1512,9 +1589,7 @@
       <c r="R6" s="3">
         <v>159</v>
       </c>
-      <c r="S6" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="S6" s="3"/>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
       <c r="V6" s="3"/>
@@ -1522,10 +1597,10 @@
       <c r="X6" s="3"/>
       <c r="Y6" s="3"/>
       <c r="Z6" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AA6" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB6" s="3"/>
     </row>
@@ -1573,7 +1648,7 @@
         <v>56</v>
       </c>
       <c r="O7" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
@@ -1581,7 +1656,7 @@
         <v>25058</v>
       </c>
       <c r="S7" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T7" s="7"/>
       <c r="U7" s="7"/>
@@ -1590,10 +1665,10 @@
       <c r="X7" s="7"/>
       <c r="Y7" s="7"/>
       <c r="Z7" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AA7" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB7" s="7">
         <v>1</v>
@@ -1643,7 +1718,7 @@
         <v>56</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
@@ -1658,10 +1733,10 @@
       <c r="X8" s="3"/>
       <c r="Y8" s="3"/>
       <c r="Z8" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AA8" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB8" s="3"/>
     </row>
@@ -1709,7 +1784,7 @@
         <v>63</v>
       </c>
       <c r="O9" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P9" s="7"/>
       <c r="Q9" s="7"/>
@@ -1717,7 +1792,7 @@
         <v>68653</v>
       </c>
       <c r="S9" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T9" s="7"/>
       <c r="U9" s="7"/>
@@ -1726,10 +1801,10 @@
       <c r="X9" s="7"/>
       <c r="Y9" s="7"/>
       <c r="Z9" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AA9" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB9" s="7">
         <v>1</v>
@@ -1779,7 +1854,7 @@
         <v>63</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
@@ -1794,10 +1869,10 @@
       <c r="X10" s="3"/>
       <c r="Y10" s="3"/>
       <c r="Z10" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AA10" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB10" s="3"/>
     </row>
@@ -1843,7 +1918,7 @@
       </c>
       <c r="N11" s="8"/>
       <c r="O11" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P11" s="7"/>
       <c r="Q11" s="7"/>
@@ -1851,7 +1926,7 @@
         <v>28400</v>
       </c>
       <c r="S11" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T11" s="7"/>
       <c r="U11" s="7"/>
@@ -1860,10 +1935,10 @@
       <c r="X11" s="7"/>
       <c r="Y11" s="7"/>
       <c r="Z11" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AA11" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB11" s="7">
         <v>1</v>
@@ -1911,7 +1986,7 @@
       </c>
       <c r="N12" s="6"/>
       <c r="O12" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
@@ -1926,10 +2001,10 @@
       <c r="X12" s="3"/>
       <c r="Y12" s="3"/>
       <c r="Z12" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AA12" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB12" s="3"/>
     </row>
@@ -1977,7 +2052,7 @@
         <v>56</v>
       </c>
       <c r="O13" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P13" s="7"/>
       <c r="Q13" s="7">
@@ -1987,7 +2062,7 @@
         <v>302935</v>
       </c>
       <c r="S13" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T13" s="7"/>
       <c r="U13" s="7"/>
@@ -1996,10 +2071,10 @@
       <c r="X13" s="7"/>
       <c r="Y13" s="7"/>
       <c r="Z13" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AA13" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB13" s="7">
         <v>1</v>
@@ -2049,7 +2124,7 @@
         <v>56</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P14" s="3"/>
       <c r="Q14" s="3">
@@ -2066,10 +2141,10 @@
       <c r="X14" s="3"/>
       <c r="Y14" s="3"/>
       <c r="Z14" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AA14" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB14" s="3"/>
     </row>
@@ -2135,7 +2210,7 @@
         <v>84</v>
       </c>
       <c r="AA15" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB15" s="7">
         <v>1</v>
@@ -2181,7 +2256,7 @@
         <v>90</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
@@ -2189,7 +2264,7 @@
         <v>0</v>
       </c>
       <c r="S16" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T16" s="3"/>
       <c r="U16" s="3"/>
@@ -2201,7 +2276,7 @@
         <v>91</v>
       </c>
       <c r="AA16" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB16" s="3">
         <v>1</v>
@@ -2247,7 +2322,7 @@
         <v>95</v>
       </c>
       <c r="O17" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P17" s="7"/>
       <c r="Q17" s="7"/>
@@ -2255,7 +2330,7 @@
         <v>0</v>
       </c>
       <c r="S17" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T17" s="7"/>
       <c r="U17" s="7"/>
@@ -2267,7 +2342,7 @@
         <v>91</v>
       </c>
       <c r="AA17" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB17" s="7">
         <v>1</v>
@@ -2335,7 +2410,7 @@
         <v>98</v>
       </c>
       <c r="AA18" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB18" s="3">
         <v>1</v>
@@ -2381,7 +2456,7 @@
         <v>103</v>
       </c>
       <c r="O19" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P19" s="7"/>
       <c r="Q19" s="7"/>
@@ -2389,7 +2464,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T19" s="7"/>
       <c r="U19" s="7"/>
@@ -2401,7 +2476,7 @@
         <v>91</v>
       </c>
       <c r="AA19" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB19" s="7">
         <v>1</v>
@@ -2447,7 +2522,7 @@
         <v>108</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
@@ -2455,7 +2530,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T20" s="3"/>
       <c r="U20" s="3"/>
@@ -2467,7 +2542,7 @@
         <v>91</v>
       </c>
       <c r="AA20" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB20" s="3">
         <v>1</v>
@@ -2513,7 +2588,7 @@
         <v>113</v>
       </c>
       <c r="O21" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P21" s="7"/>
       <c r="Q21" s="7"/>
@@ -2521,7 +2596,7 @@
         <v>0</v>
       </c>
       <c r="S21" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T21" s="7"/>
       <c r="U21" s="7"/>
@@ -2533,7 +2608,7 @@
         <v>91</v>
       </c>
       <c r="AA21" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB21" s="7">
         <v>1</v>
@@ -2601,7 +2676,7 @@
         <v>119</v>
       </c>
       <c r="AA22" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB22" s="3">
         <v>1</v>
@@ -2647,7 +2722,7 @@
         <v>118</v>
       </c>
       <c r="O23" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P23" s="7"/>
       <c r="Q23" s="7"/>
@@ -2655,7 +2730,7 @@
         <v>0</v>
       </c>
       <c r="S23" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T23" s="7"/>
       <c r="U23" s="7"/>
@@ -2667,7 +2742,7 @@
         <v>91</v>
       </c>
       <c r="AA23" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB23" s="7"/>
     </row>
@@ -2676,7 +2751,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="3">
-        <v>2025100333</v>
+        <v>2025100602</v>
       </c>
       <c r="C24" s="3">
         <v>1</v>
@@ -2688,56 +2763,54 @@
         <v>122</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>85</v>
+        <v>123</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>123</v>
+        <v>44</v>
       </c>
       <c r="H24" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I24" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="J24" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>126</v>
       </c>
       <c r="K24" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L24" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="M24" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="M24" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="N24" s="6" t="s">
-        <v>129</v>
-      </c>
+      <c r="N24" s="6"/>
       <c r="O24" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P24" s="3"/>
       <c r="Q24" s="3">
-        <v>16366</v>
+        <v>2150</v>
       </c>
       <c r="R24" s="3">
-        <v>143510</v>
-      </c>
-      <c r="S24" s="3"/>
+        <v>43000</v>
+      </c>
+      <c r="S24" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="T24" s="3"/>
-      <c r="U24" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="U24" s="3"/>
       <c r="V24" s="3"/>
       <c r="W24" s="3"/>
       <c r="X24" s="3"/>
       <c r="Y24" s="3"/>
       <c r="Z24" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="AA24" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB24" s="3">
         <v>1</v>
@@ -2748,7 +2821,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="7">
-        <v>2025100335</v>
+        <v>2025100603</v>
       </c>
       <c r="C25" s="7">
         <v>1</v>
@@ -2760,67 +2833,61 @@
         <v>122</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>85</v>
+        <v>123</v>
       </c>
       <c r="G25" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="I25" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="H25" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>132</v>
-      </c>
       <c r="J25" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K25" s="7" t="s">
         <v>36</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="M25" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="N25" s="8" t="s">
-        <v>135</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="N25" s="8"/>
       <c r="O25" s="7" t="s">
         <v>40</v>
       </c>
       <c r="P25" s="7"/>
       <c r="Q25" s="7">
-        <v>5983</v>
+        <v>2150</v>
       </c>
       <c r="R25" s="7">
-        <v>32582</v>
+        <v>43000</v>
       </c>
       <c r="S25" s="7"/>
       <c r="T25" s="7"/>
-      <c r="U25" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="U25" s="7"/>
       <c r="V25" s="7"/>
       <c r="W25" s="7"/>
       <c r="X25" s="7"/>
       <c r="Y25" s="7"/>
       <c r="Z25" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="AA25" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB25" s="7">
-        <v>1</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="AB25" s="7"/>
     </row>
     <row r="26" spans="1:28">
       <c r="A26" s="3">
         <v>24</v>
       </c>
       <c r="B26" s="3">
-        <v>2025100077</v>
+        <v>2025100333</v>
       </c>
       <c r="C26" s="3">
         <v>1</v>
@@ -2832,63 +2899,67 @@
         <v>122</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>50</v>
+        <v>129</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>35</v>
+        <v>125</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L26" s="6" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="M26" s="6" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="N26" s="6" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P26" s="3"/>
       <c r="Q26" s="3">
-        <v>843</v>
+        <v>16366</v>
       </c>
       <c r="R26" s="3">
-        <v>44687</v>
-      </c>
-      <c r="S26" s="3" t="s">
-        <v>41</v>
-      </c>
+        <v>143510</v>
+      </c>
+      <c r="S26" s="3"/>
       <c r="T26" s="3"/>
-      <c r="U26" s="3"/>
+      <c r="U26" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="V26" s="3"/>
       <c r="W26" s="3"/>
       <c r="X26" s="3"/>
       <c r="Y26" s="3"/>
       <c r="Z26" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA26" s="3"/>
-      <c r="AB26" s="3"/>
+        <v>135</v>
+      </c>
+      <c r="AA26" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB26" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:28">
       <c r="A27" s="7">
         <v>25</v>
       </c>
       <c r="B27" s="7">
-        <v>2025100078</v>
+        <v>2025100335</v>
       </c>
       <c r="C27" s="7">
         <v>1</v>
@@ -2900,10 +2971,10 @@
         <v>122</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="H27" s="7" t="s">
         <v>136</v>
@@ -2912,7 +2983,7 @@
         <v>137</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>35</v>
+        <v>125</v>
       </c>
       <c r="K27" s="7" t="s">
         <v>36</v>
@@ -2931,32 +3002,36 @@
       </c>
       <c r="P27" s="7"/>
       <c r="Q27" s="7">
-        <v>843</v>
+        <v>5983</v>
       </c>
       <c r="R27" s="7">
-        <v>44687</v>
+        <v>32582</v>
       </c>
       <c r="S27" s="7"/>
       <c r="T27" s="7"/>
-      <c r="U27" s="7"/>
+      <c r="U27" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="V27" s="7"/>
       <c r="W27" s="7"/>
       <c r="X27" s="7"/>
       <c r="Y27" s="7"/>
       <c r="Z27" s="8" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="AA27" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB27" s="7"/>
+        <v>42</v>
+      </c>
+      <c r="AB27" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:28">
       <c r="A28" s="3">
         <v>26</v>
       </c>
       <c r="B28" s="3">
-        <v>2025100454</v>
+        <v>2025100597</v>
       </c>
       <c r="C28" s="3">
         <v>1</v>
@@ -2968,16 +3043,16 @@
         <v>122</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>85</v>
+        <v>123</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>105</v>
+        <v>136</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>35</v>
@@ -2986,25 +3061,27 @@
         <v>36</v>
       </c>
       <c r="L28" s="6" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="N28" s="6" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="O28" s="3" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="P28" s="3"/>
       <c r="Q28" s="3">
-        <v>843</v>
+        <v>900</v>
       </c>
       <c r="R28" s="3">
-        <v>44687</v>
-      </c>
-      <c r="S28" s="3"/>
+        <v>13500</v>
+      </c>
+      <c r="S28" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="T28" s="3"/>
       <c r="U28" s="3"/>
       <c r="V28" s="3"/>
@@ -3012,10 +3089,10 @@
       <c r="X28" s="3"/>
       <c r="Y28" s="3"/>
       <c r="Z28" s="6" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="AA28" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB28" s="3">
         <v>1</v>
@@ -3026,7 +3103,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="7">
-        <v>2025100084</v>
+        <v>2025100598</v>
       </c>
       <c r="C29" s="7">
         <v>1</v>
@@ -3038,16 +3115,16 @@
         <v>122</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>31</v>
+        <v>123</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>144</v>
+        <v>92</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="J29" s="7" t="s">
         <v>35</v>
@@ -3056,27 +3133,25 @@
         <v>36</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>47</v>
+        <v>142</v>
       </c>
       <c r="M29" s="8" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="N29" s="8" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="O29" s="7" t="s">
         <v>40</v>
       </c>
       <c r="P29" s="7"/>
       <c r="Q29" s="7">
-        <v>56</v>
+        <v>900</v>
       </c>
       <c r="R29" s="7">
-        <v>400</v>
-      </c>
-      <c r="S29" s="7" t="s">
-        <v>41</v>
-      </c>
+        <v>13500</v>
+      </c>
+      <c r="S29" s="7"/>
       <c r="T29" s="7"/>
       <c r="U29" s="7"/>
       <c r="V29" s="7"/>
@@ -3084,21 +3159,19 @@
       <c r="X29" s="7"/>
       <c r="Y29" s="7"/>
       <c r="Z29" s="8" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="AA29" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB29" s="7">
-        <v>1</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="AB29" s="7"/>
     </row>
     <row r="30" spans="1:28">
       <c r="A30" s="3">
         <v>28</v>
       </c>
       <c r="B30" s="3">
-        <v>2025100085</v>
+        <v>2025100077</v>
       </c>
       <c r="C30" s="3">
         <v>1</v>
@@ -3113,13 +3186,13 @@
         <v>31</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>143</v>
+        <v>50</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="J30" s="3" t="s">
         <v>35</v>
@@ -3128,25 +3201,27 @@
         <v>36</v>
       </c>
       <c r="L30" s="6" t="s">
-        <v>47</v>
+        <v>147</v>
       </c>
       <c r="M30" s="6" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="N30" s="6" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="O30" s="3" t="s">
         <v>43</v>
       </c>
       <c r="P30" s="3"/>
       <c r="Q30" s="3">
-        <v>56</v>
+        <v>843</v>
       </c>
       <c r="R30" s="3">
-        <v>400</v>
-      </c>
-      <c r="S30" s="3"/>
+        <v>44687</v>
+      </c>
+      <c r="S30" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="T30" s="3"/>
       <c r="U30" s="3"/>
       <c r="V30" s="3"/>
@@ -3154,11 +3229,9 @@
       <c r="X30" s="3"/>
       <c r="Y30" s="3"/>
       <c r="Z30" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA30" s="3" t="s">
-        <v>41</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="AA30" s="3"/>
       <c r="AB30" s="3"/>
     </row>
     <row r="31" spans="1:28">
@@ -3166,7 +3239,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="7">
-        <v>2025100074</v>
+        <v>2025100078</v>
       </c>
       <c r="C31" s="7">
         <v>1</v>
@@ -3181,40 +3254,40 @@
         <v>31</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>148</v>
+        <v>50</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="K31" s="7" t="s">
         <v>36</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="M31" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="N31" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="O31" s="7" t="s">
         <v>40</v>
       </c>
       <c r="P31" s="7"/>
-      <c r="Q31" s="7"/>
+      <c r="Q31" s="7">
+        <v>843</v>
+      </c>
       <c r="R31" s="7">
-        <v>193</v>
-      </c>
-      <c r="S31" s="7" t="s">
-        <v>41</v>
-      </c>
+        <v>44687</v>
+      </c>
+      <c r="S31" s="7"/>
       <c r="T31" s="7"/>
       <c r="U31" s="7"/>
       <c r="V31" s="7"/>
@@ -3222,21 +3295,19 @@
       <c r="X31" s="7"/>
       <c r="Y31" s="7"/>
       <c r="Z31" s="8" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="AA31" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB31" s="7">
-        <v>1</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="AB31" s="7"/>
     </row>
     <row r="32" spans="1:28">
       <c r="A32" s="3">
         <v>30</v>
       </c>
       <c r="B32" s="3">
-        <v>2025100075</v>
+        <v>2025100454</v>
       </c>
       <c r="C32" s="3">
         <v>1</v>
@@ -3248,39 +3319,41 @@
         <v>122</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>148</v>
+        <v>105</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="K32" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L32" s="6" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="M32" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="N32" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="O32" s="3" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="P32" s="3"/>
-      <c r="Q32" s="3"/>
+      <c r="Q32" s="3">
+        <v>843</v>
+      </c>
       <c r="R32" s="3">
-        <v>193</v>
+        <v>44687</v>
       </c>
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
@@ -3290,19 +3363,21 @@
       <c r="X32" s="3"/>
       <c r="Y32" s="3"/>
       <c r="Z32" s="6" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="AA32" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB32" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="AB32" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="1:28">
       <c r="A33" s="7">
         <v>31</v>
       </c>
       <c r="B33" s="7">
-        <v>2025100368</v>
+        <v>2025100084</v>
       </c>
       <c r="C33" s="7">
         <v>1</v>
@@ -3314,42 +3389,44 @@
         <v>122</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>92</v>
+        <v>151</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>44</v>
+        <v>152</v>
       </c>
       <c r="I33" s="7" t="s">
         <v>153</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="K33" s="7" t="s">
         <v>36</v>
       </c>
       <c r="L33" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="M33" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="M33" s="8" t="s">
-        <v>155</v>
-      </c>
       <c r="N33" s="8" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="O33" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P33" s="7"/>
-      <c r="Q33" s="7"/>
+      <c r="Q33" s="7">
+        <v>56</v>
+      </c>
       <c r="R33" s="7">
-        <v>155192</v>
+        <v>400</v>
       </c>
       <c r="S33" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T33" s="7"/>
       <c r="U33" s="7"/>
@@ -3358,10 +3435,10 @@
       <c r="X33" s="7"/>
       <c r="Y33" s="7"/>
       <c r="Z33" s="8" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="AA33" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB33" s="7">
         <v>1</v>
@@ -3372,7 +3449,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="3">
-        <v>2025100369</v>
+        <v>2025100085</v>
       </c>
       <c r="C34" s="3">
         <v>1</v>
@@ -3384,39 +3461,41 @@
         <v>122</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>92</v>
+        <v>151</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>44</v>
+        <v>152</v>
       </c>
       <c r="I34" s="3" t="s">
         <v>153</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="K34" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L34" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="M34" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="M34" s="6" t="s">
-        <v>155</v>
-      </c>
       <c r="N34" s="6" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="O34" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P34" s="3"/>
-      <c r="Q34" s="3"/>
+      <c r="Q34" s="3">
+        <v>56</v>
+      </c>
       <c r="R34" s="3">
-        <v>155192</v>
+        <v>400</v>
       </c>
       <c r="S34" s="3"/>
       <c r="T34" s="3"/>
@@ -3426,10 +3505,10 @@
       <c r="X34" s="3"/>
       <c r="Y34" s="3"/>
       <c r="Z34" s="6" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="AA34" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB34" s="3"/>
     </row>
@@ -3438,7 +3517,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="7">
-        <v>2025100371</v>
+        <v>2025100074</v>
       </c>
       <c r="C35" s="7">
         <v>1</v>
@@ -3450,25 +3529,25 @@
         <v>122</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>44</v>
+        <v>155</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="K35" s="7" t="s">
         <v>36</v>
       </c>
       <c r="L35" s="8" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="M35" s="8" t="s">
         <v>158</v>
@@ -3482,9 +3561,11 @@
       <c r="P35" s="7"/>
       <c r="Q35" s="7"/>
       <c r="R35" s="7">
-        <v>140987</v>
-      </c>
-      <c r="S35" s="7"/>
+        <v>193</v>
+      </c>
+      <c r="S35" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="T35" s="7"/>
       <c r="U35" s="7"/>
       <c r="V35" s="7"/>
@@ -3492,10 +3573,10 @@
       <c r="X35" s="7"/>
       <c r="Y35" s="7"/>
       <c r="Z35" s="8" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="AA35" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB35" s="7">
         <v>1</v>
@@ -3506,7 +3587,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="3">
-        <v>2025100370</v>
+        <v>2025100075</v>
       </c>
       <c r="C36" s="3">
         <v>1</v>
@@ -3518,25 +3599,25 @@
         <v>122</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>44</v>
+        <v>155</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="K36" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L36" s="6" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="M36" s="6" t="s">
         <v>158</v>
@@ -3550,11 +3631,9 @@
       <c r="P36" s="3"/>
       <c r="Q36" s="3"/>
       <c r="R36" s="3">
-        <v>140987</v>
-      </c>
-      <c r="S36" s="3" t="s">
-        <v>41</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="S36" s="3"/>
       <c r="T36" s="3"/>
       <c r="U36" s="3"/>
       <c r="V36" s="3"/>
@@ -3562,10 +3641,10 @@
       <c r="X36" s="3"/>
       <c r="Y36" s="3"/>
       <c r="Z36" s="6" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="AA36" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB36" s="3"/>
     </row>
@@ -3574,7 +3653,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="7">
-        <v>2025100502</v>
+        <v>2025100368</v>
       </c>
       <c r="C37" s="7">
         <v>1</v>
@@ -3589,10 +3668,10 @@
         <v>85</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>136</v>
+        <v>92</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>143</v>
+        <v>44</v>
       </c>
       <c r="I37" s="7" t="s">
         <v>160</v>
@@ -3613,15 +3692,15 @@
         <v>163</v>
       </c>
       <c r="O37" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P37" s="7"/>
       <c r="Q37" s="7"/>
       <c r="R37" s="7">
-        <v>299683</v>
+        <v>155192</v>
       </c>
       <c r="S37" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T37" s="7"/>
       <c r="U37" s="7"/>
@@ -3630,17 +3709,21 @@
       <c r="X37" s="7"/>
       <c r="Y37" s="7"/>
       <c r="Z37" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA37" s="7"/>
-      <c r="AB37" s="7"/>
+        <v>128</v>
+      </c>
+      <c r="AA37" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB37" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="38" spans="1:28">
       <c r="A38" s="3">
         <v>36</v>
       </c>
       <c r="B38" s="3">
-        <v>2025100503</v>
+        <v>2025100369</v>
       </c>
       <c r="C38" s="3">
         <v>1</v>
@@ -3655,10 +3738,10 @@
         <v>85</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>136</v>
+        <v>92</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>143</v>
+        <v>44</v>
       </c>
       <c r="I38" s="3" t="s">
         <v>160</v>
@@ -3679,12 +3762,12 @@
         <v>163</v>
       </c>
       <c r="O38" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P38" s="3"/>
       <c r="Q38" s="3"/>
       <c r="R38" s="3">
-        <v>299683</v>
+        <v>155192</v>
       </c>
       <c r="S38" s="3"/>
       <c r="T38" s="3"/>
@@ -3694,10 +3777,10 @@
       <c r="X38" s="3"/>
       <c r="Y38" s="3"/>
       <c r="Z38" s="6" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="AA38" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB38" s="3"/>
     </row>
@@ -3706,7 +3789,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="7">
-        <v>2025100498</v>
+        <v>2025100371</v>
       </c>
       <c r="C39" s="7">
         <v>1</v>
@@ -3721,10 +3804,10 @@
         <v>85</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>136</v>
+        <v>96</v>
       </c>
       <c r="I39" s="7" t="s">
         <v>164</v>
@@ -3750,11 +3833,9 @@
       <c r="P39" s="7"/>
       <c r="Q39" s="7"/>
       <c r="R39" s="7">
-        <v>240934</v>
-      </c>
-      <c r="S39" s="7" t="s">
-        <v>41</v>
-      </c>
+        <v>140987</v>
+      </c>
+      <c r="S39" s="7"/>
       <c r="T39" s="7"/>
       <c r="U39" s="7"/>
       <c r="V39" s="7"/>
@@ -3762,17 +3843,21 @@
       <c r="X39" s="7"/>
       <c r="Y39" s="7"/>
       <c r="Z39" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA39" s="7"/>
-      <c r="AB39" s="7"/>
+        <v>128</v>
+      </c>
+      <c r="AA39" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB39" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="40" spans="1:28">
       <c r="A40" s="3">
         <v>38</v>
       </c>
       <c r="B40" s="3">
-        <v>2025100499</v>
+        <v>2025100370</v>
       </c>
       <c r="C40" s="3">
         <v>1</v>
@@ -3787,10 +3872,10 @@
         <v>85</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>136</v>
+        <v>96</v>
       </c>
       <c r="I40" s="3" t="s">
         <v>164</v>
@@ -3816,9 +3901,11 @@
       <c r="P40" s="3"/>
       <c r="Q40" s="3"/>
       <c r="R40" s="3">
-        <v>240934</v>
-      </c>
-      <c r="S40" s="3"/>
+        <v>140987</v>
+      </c>
+      <c r="S40" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="T40" s="3"/>
       <c r="U40" s="3"/>
       <c r="V40" s="3"/>
@@ -3826,10 +3913,10 @@
       <c r="X40" s="3"/>
       <c r="Y40" s="3"/>
       <c r="Z40" s="6" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="AA40" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB40" s="3"/>
     </row>
@@ -3838,7 +3925,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="7">
-        <v>2025100070</v>
+        <v>2025100599</v>
       </c>
       <c r="C41" s="7">
         <v>1</v>
@@ -3850,13 +3937,13 @@
         <v>122</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>31</v>
+        <v>123</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>97</v>
+        <v>44</v>
       </c>
       <c r="I41" s="7" t="s">
         <v>167</v>
@@ -3868,24 +3955,22 @@
         <v>36</v>
       </c>
       <c r="L41" s="8" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="M41" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="N41" s="8" t="s">
         <v>169</v>
       </c>
+      <c r="N41" s="8"/>
       <c r="O41" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P41" s="7"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="7">
-        <v>4020</v>
+        <v>50000</v>
       </c>
       <c r="S41" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T41" s="7"/>
       <c r="U41" s="7"/>
@@ -3894,10 +3979,10 @@
       <c r="X41" s="7"/>
       <c r="Y41" s="7"/>
       <c r="Z41" s="8" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="AA41" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB41" s="7">
         <v>1</v>
@@ -3908,7 +3993,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="3">
-        <v>2025100071</v>
+        <v>2025100600</v>
       </c>
       <c r="C42" s="3">
         <v>1</v>
@@ -3920,13 +4005,13 @@
         <v>122</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>31</v>
+        <v>123</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>97</v>
+        <v>44</v>
       </c>
       <c r="I42" s="3" t="s">
         <v>167</v>
@@ -3938,21 +4023,19 @@
         <v>36</v>
       </c>
       <c r="L42" s="6" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="M42" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="N42" s="6" t="s">
         <v>169</v>
       </c>
+      <c r="N42" s="6"/>
       <c r="O42" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P42" s="3"/>
       <c r="Q42" s="3"/>
       <c r="R42" s="3">
-        <v>4020</v>
+        <v>50000</v>
       </c>
       <c r="S42" s="3"/>
       <c r="T42" s="3"/>
@@ -3962,10 +4045,10 @@
       <c r="X42" s="3"/>
       <c r="Y42" s="3"/>
       <c r="Z42" s="6" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="AA42" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB42" s="3"/>
     </row>
@@ -3974,7 +4057,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="7">
-        <v>2025100065</v>
+        <v>2025100502</v>
       </c>
       <c r="C43" s="7">
         <v>1</v>
@@ -3986,13 +4069,13 @@
         <v>122</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>92</v>
+        <v>145</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>44</v>
+        <v>151</v>
       </c>
       <c r="I43" s="7" t="s">
         <v>170</v>
@@ -4004,24 +4087,24 @@
         <v>36</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>150</v>
+        <v>171</v>
       </c>
       <c r="M43" s="8" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="N43" s="8" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="O43" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P43" s="7"/>
       <c r="Q43" s="7"/>
       <c r="R43" s="7">
-        <v>5001</v>
+        <v>299683</v>
       </c>
       <c r="S43" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T43" s="7"/>
       <c r="U43" s="7"/>
@@ -4030,21 +4113,17 @@
       <c r="X43" s="7"/>
       <c r="Y43" s="7"/>
       <c r="Z43" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA43" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB43" s="7">
-        <v>1</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="AA43" s="7"/>
+      <c r="AB43" s="7"/>
     </row>
     <row r="44" spans="1:28">
       <c r="A44" s="3">
         <v>42</v>
       </c>
       <c r="B44" s="3">
-        <v>2025100066</v>
+        <v>2025100503</v>
       </c>
       <c r="C44" s="3">
         <v>1</v>
@@ -4056,13 +4135,13 @@
         <v>122</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>92</v>
+        <v>145</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>44</v>
+        <v>151</v>
       </c>
       <c r="I44" s="3" t="s">
         <v>170</v>
@@ -4074,21 +4153,21 @@
         <v>36</v>
       </c>
       <c r="L44" s="6" t="s">
-        <v>150</v>
+        <v>171</v>
       </c>
       <c r="M44" s="6" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="N44" s="6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="O44" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P44" s="3"/>
       <c r="Q44" s="3"/>
       <c r="R44" s="3">
-        <v>5001</v>
+        <v>299683</v>
       </c>
       <c r="S44" s="3"/>
       <c r="T44" s="3"/>
@@ -4098,10 +4177,10 @@
       <c r="X44" s="3"/>
       <c r="Y44" s="3"/>
       <c r="Z44" s="6" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="AA44" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB44" s="3"/>
     </row>
@@ -4110,7 +4189,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="7">
-        <v>2025100059</v>
+        <v>2025100498</v>
       </c>
       <c r="C45" s="7">
         <v>1</v>
@@ -4122,16 +4201,16 @@
         <v>122</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>123</v>
+        <v>50</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>124</v>
+        <v>145</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J45" s="7" t="s">
         <v>60</v>
@@ -4140,24 +4219,24 @@
         <v>36</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>150</v>
+        <v>171</v>
       </c>
       <c r="M45" s="8" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="N45" s="8" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="O45" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P45" s="7"/>
       <c r="Q45" s="7"/>
       <c r="R45" s="7">
-        <v>3173</v>
+        <v>240934</v>
       </c>
       <c r="S45" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T45" s="7"/>
       <c r="U45" s="7"/>
@@ -4166,21 +4245,17 @@
       <c r="X45" s="7"/>
       <c r="Y45" s="7"/>
       <c r="Z45" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA45" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB45" s="7">
-        <v>1</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="AA45" s="7"/>
+      <c r="AB45" s="7"/>
     </row>
     <row r="46" spans="1:28">
       <c r="A46" s="3">
         <v>44</v>
       </c>
       <c r="B46" s="3">
-        <v>2025100060</v>
+        <v>2025100499</v>
       </c>
       <c r="C46" s="3">
         <v>1</v>
@@ -4192,16 +4267,16 @@
         <v>122</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>123</v>
+        <v>50</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>124</v>
+        <v>145</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J46" s="3" t="s">
         <v>60</v>
@@ -4210,21 +4285,21 @@
         <v>36</v>
       </c>
       <c r="L46" s="6" t="s">
-        <v>150</v>
+        <v>171</v>
       </c>
       <c r="M46" s="6" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="N46" s="6" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="O46" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P46" s="3"/>
       <c r="Q46" s="3"/>
       <c r="R46" s="3">
-        <v>3173</v>
+        <v>240934</v>
       </c>
       <c r="S46" s="3"/>
       <c r="T46" s="3"/>
@@ -4234,10 +4309,10 @@
       <c r="X46" s="3"/>
       <c r="Y46" s="3"/>
       <c r="Z46" s="6" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="AA46" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB46" s="3"/>
     </row>
@@ -4246,7 +4321,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="7">
-        <v>2025100063</v>
+        <v>2025100070</v>
       </c>
       <c r="C47" s="7">
         <v>1</v>
@@ -4261,13 +4336,13 @@
         <v>31</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>131</v>
+        <v>96</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="J47" s="7" t="s">
         <v>60</v>
@@ -4276,24 +4351,24 @@
         <v>36</v>
       </c>
       <c r="L47" s="8" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="M47" s="8" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="N47" s="8" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="O47" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P47" s="7"/>
       <c r="Q47" s="7"/>
       <c r="R47" s="7">
-        <v>2841</v>
+        <v>4020</v>
       </c>
       <c r="S47" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T47" s="7"/>
       <c r="U47" s="7"/>
@@ -4302,10 +4377,10 @@
       <c r="X47" s="7"/>
       <c r="Y47" s="7"/>
       <c r="Z47" s="8" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="AA47" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB47" s="7">
         <v>1</v>
@@ -4316,7 +4391,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="3">
-        <v>2025100064</v>
+        <v>2025100071</v>
       </c>
       <c r="C48" s="3">
         <v>1</v>
@@ -4331,13 +4406,13 @@
         <v>31</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>131</v>
+        <v>96</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="J48" s="3" t="s">
         <v>60</v>
@@ -4346,21 +4421,21 @@
         <v>36</v>
       </c>
       <c r="L48" s="6" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="M48" s="6" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="N48" s="6" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="O48" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P48" s="3"/>
       <c r="Q48" s="3"/>
       <c r="R48" s="3">
-        <v>2841</v>
+        <v>4020</v>
       </c>
       <c r="S48" s="3"/>
       <c r="T48" s="3"/>
@@ -4370,10 +4445,10 @@
       <c r="X48" s="3"/>
       <c r="Y48" s="3"/>
       <c r="Z48" s="6" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="AA48" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB48" s="3"/>
     </row>
@@ -4382,7 +4457,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="7">
-        <v>2025100061</v>
+        <v>2025100065</v>
       </c>
       <c r="C49" s="7">
         <v>1</v>
@@ -4397,13 +4472,13 @@
         <v>31</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>131</v>
+        <v>44</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J49" s="7" t="s">
         <v>60</v>
@@ -4412,24 +4487,24 @@
         <v>36</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="M49" s="8" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="N49" s="8" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="O49" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P49" s="7"/>
       <c r="Q49" s="7"/>
       <c r="R49" s="7">
-        <v>1935</v>
+        <v>5001</v>
       </c>
       <c r="S49" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T49" s="7"/>
       <c r="U49" s="7"/>
@@ -4438,10 +4513,10 @@
       <c r="X49" s="7"/>
       <c r="Y49" s="7"/>
       <c r="Z49" s="8" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="AA49" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB49" s="7">
         <v>1</v>
@@ -4452,7 +4527,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="3">
-        <v>2025100062</v>
+        <v>2025100066</v>
       </c>
       <c r="C50" s="3">
         <v>1</v>
@@ -4467,13 +4542,13 @@
         <v>31</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>131</v>
+        <v>44</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J50" s="3" t="s">
         <v>60</v>
@@ -4482,21 +4557,21 @@
         <v>36</v>
       </c>
       <c r="L50" s="6" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="M50" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="N50" s="6" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="O50" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P50" s="3"/>
       <c r="Q50" s="3"/>
       <c r="R50" s="3">
-        <v>1935</v>
+        <v>5001</v>
       </c>
       <c r="S50" s="3"/>
       <c r="T50" s="3"/>
@@ -4506,10 +4581,10 @@
       <c r="X50" s="3"/>
       <c r="Y50" s="3"/>
       <c r="Z50" s="6" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="AA50" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB50" s="3"/>
     </row>
@@ -4518,7 +4593,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="7">
-        <v>2025100336</v>
+        <v>2025100059</v>
       </c>
       <c r="C51" s="7">
         <v>1</v>
@@ -4530,25 +4605,25 @@
         <v>122</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>92</v>
+        <v>130</v>
       </c>
       <c r="I51" s="7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="J51" s="7" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="K51" s="7" t="s">
         <v>36</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>183</v>
+        <v>157</v>
       </c>
       <c r="M51" s="8" t="s">
         <v>184</v>
@@ -4557,29 +4632,27 @@
         <v>185</v>
       </c>
       <c r="O51" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P51" s="7"/>
-      <c r="Q51" s="7">
-        <v>28805</v>
-      </c>
+      <c r="Q51" s="7"/>
       <c r="R51" s="7">
-        <v>28881</v>
-      </c>
-      <c r="S51" s="7"/>
+        <v>3173</v>
+      </c>
+      <c r="S51" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="T51" s="7"/>
-      <c r="U51" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="U51" s="7"/>
       <c r="V51" s="7"/>
       <c r="W51" s="7"/>
       <c r="X51" s="7"/>
       <c r="Y51" s="7"/>
       <c r="Z51" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="AA51" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB51" s="7">
         <v>1</v>
@@ -4590,7 +4663,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="3">
-        <v>2025100516</v>
+        <v>2025100060</v>
       </c>
       <c r="C52" s="3">
         <v>1</v>
@@ -4602,31 +4675,31 @@
         <v>122</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>186</v>
+        <v>129</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>105</v>
+        <v>130</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>188</v>
+        <v>60</v>
       </c>
       <c r="K52" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L52" s="6" t="s">
-        <v>189</v>
+        <v>157</v>
       </c>
       <c r="M52" s="6" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="N52" s="6" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="O52" s="3" t="s">
         <v>40</v>
@@ -4634,11 +4707,9 @@
       <c r="P52" s="3"/>
       <c r="Q52" s="3"/>
       <c r="R52" s="3">
-        <v>297956</v>
-      </c>
-      <c r="S52" s="3" t="s">
-        <v>41</v>
-      </c>
+        <v>3173</v>
+      </c>
+      <c r="S52" s="3"/>
       <c r="T52" s="3"/>
       <c r="U52" s="3"/>
       <c r="V52" s="3"/>
@@ -4646,9 +4717,11 @@
       <c r="X52" s="3"/>
       <c r="Y52" s="3"/>
       <c r="Z52" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA52" s="3"/>
+        <v>128</v>
+      </c>
+      <c r="AA52" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="AB52" s="3"/>
     </row>
     <row r="53" spans="1:28">
@@ -4656,7 +4729,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="7">
-        <v>2025100517</v>
+        <v>2025100063</v>
       </c>
       <c r="C53" s="7">
         <v>1</v>
@@ -4668,31 +4741,31 @@
         <v>122</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
       <c r="G53" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="H53" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I53" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="H53" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="I53" s="7" t="s">
-        <v>187</v>
-      </c>
       <c r="J53" s="7" t="s">
-        <v>188</v>
+        <v>60</v>
       </c>
       <c r="K53" s="7" t="s">
         <v>36</v>
       </c>
       <c r="L53" s="8" t="s">
-        <v>189</v>
+        <v>157</v>
       </c>
       <c r="M53" s="8" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="N53" s="8" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="O53" s="7" t="s">
         <v>43</v>
@@ -4700,9 +4773,11 @@
       <c r="P53" s="7"/>
       <c r="Q53" s="7"/>
       <c r="R53" s="7">
-        <v>297956</v>
-      </c>
-      <c r="S53" s="7"/>
+        <v>2841</v>
+      </c>
+      <c r="S53" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="T53" s="7"/>
       <c r="U53" s="7"/>
       <c r="V53" s="7"/>
@@ -4710,19 +4785,21 @@
       <c r="X53" s="7"/>
       <c r="Y53" s="7"/>
       <c r="Z53" s="8" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="AA53" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB53" s="7"/>
+        <v>42</v>
+      </c>
+      <c r="AB53" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="54" spans="1:28">
       <c r="A54" s="3">
         <v>52</v>
       </c>
       <c r="B54" s="3">
-        <v>2025100511</v>
+        <v>2025100064</v>
       </c>
       <c r="C54" s="3">
         <v>1</v>
@@ -4734,31 +4811,31 @@
         <v>122</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>87</v>
+        <v>136</v>
       </c>
       <c r="H54" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I54" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="I54" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="J54" s="3" t="s">
-        <v>188</v>
+        <v>60</v>
       </c>
       <c r="K54" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L54" s="6" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="M54" s="6" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="N54" s="6" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="O54" s="3" t="s">
         <v>40</v>
@@ -4766,11 +4843,9 @@
       <c r="P54" s="3"/>
       <c r="Q54" s="3"/>
       <c r="R54" s="3">
-        <v>117288</v>
-      </c>
-      <c r="S54" s="3" t="s">
-        <v>41</v>
-      </c>
+        <v>2841</v>
+      </c>
+      <c r="S54" s="3"/>
       <c r="T54" s="3"/>
       <c r="U54" s="3"/>
       <c r="V54" s="3"/>
@@ -4778,9 +4853,11 @@
       <c r="X54" s="3"/>
       <c r="Y54" s="3"/>
       <c r="Z54" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA54" s="3"/>
+        <v>128</v>
+      </c>
+      <c r="AA54" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="AB54" s="3"/>
     </row>
     <row r="55" spans="1:28">
@@ -4788,7 +4865,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="7">
-        <v>2025100512</v>
+        <v>2025100061</v>
       </c>
       <c r="C55" s="7">
         <v>1</v>
@@ -4800,31 +4877,31 @@
         <v>122</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>87</v>
+        <v>130</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>186</v>
+        <v>136</v>
       </c>
       <c r="I55" s="7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="J55" s="7" t="s">
-        <v>188</v>
+        <v>60</v>
       </c>
       <c r="K55" s="7" t="s">
         <v>36</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="M55" s="8" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="N55" s="8" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="O55" s="7" t="s">
         <v>43</v>
@@ -4832,9 +4909,11 @@
       <c r="P55" s="7"/>
       <c r="Q55" s="7"/>
       <c r="R55" s="7">
-        <v>117288</v>
-      </c>
-      <c r="S55" s="7"/>
+        <v>1935</v>
+      </c>
+      <c r="S55" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="T55" s="7"/>
       <c r="U55" s="7"/>
       <c r="V55" s="7"/>
@@ -4842,19 +4921,21 @@
       <c r="X55" s="7"/>
       <c r="Y55" s="7"/>
       <c r="Z55" s="8" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="AA55" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB55" s="7"/>
+        <v>42</v>
+      </c>
+      <c r="AB55" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="56" spans="1:28">
       <c r="A56" s="3">
         <v>54</v>
       </c>
       <c r="B56" s="3">
-        <v>2025100072</v>
+        <v>2025100062</v>
       </c>
       <c r="C56" s="3">
         <v>1</v>
@@ -4869,28 +4950,28 @@
         <v>31</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>97</v>
+        <v>130</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>188</v>
+        <v>60</v>
       </c>
       <c r="K56" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L56" s="6" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="M56" s="6" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="N56" s="6" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="O56" s="3" t="s">
         <v>40</v>
@@ -4898,11 +4979,9 @@
       <c r="P56" s="3"/>
       <c r="Q56" s="3"/>
       <c r="R56" s="3">
-        <v>54</v>
-      </c>
-      <c r="S56" s="3" t="s">
-        <v>41</v>
-      </c>
+        <v>1935</v>
+      </c>
+      <c r="S56" s="3"/>
       <c r="T56" s="3"/>
       <c r="U56" s="3"/>
       <c r="V56" s="3"/>
@@ -4910,21 +4989,19 @@
       <c r="X56" s="3"/>
       <c r="Y56" s="3"/>
       <c r="Z56" s="6" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="AA56" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB56" s="3">
-        <v>1</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="AB56" s="3"/>
     </row>
     <row r="57" spans="1:28">
       <c r="A57" s="7">
         <v>55</v>
       </c>
       <c r="B57" s="7">
-        <v>2025100073</v>
+        <v>2025100336</v>
       </c>
       <c r="C57" s="7">
         <v>1</v>
@@ -4936,61 +5013,67 @@
         <v>122</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>97</v>
+        <v>136</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>148</v>
+        <v>92</v>
       </c>
       <c r="I57" s="7" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="J57" s="7" t="s">
-        <v>188</v>
+        <v>72</v>
       </c>
       <c r="K57" s="7" t="s">
         <v>36</v>
       </c>
       <c r="L57" s="8" t="s">
-        <v>150</v>
+        <v>193</v>
       </c>
       <c r="M57" s="8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="N57" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="O57" s="7" t="s">
         <v>43</v>
       </c>
       <c r="P57" s="7"/>
-      <c r="Q57" s="7"/>
+      <c r="Q57" s="7">
+        <v>28805</v>
+      </c>
       <c r="R57" s="7">
-        <v>54</v>
+        <v>28881</v>
       </c>
       <c r="S57" s="7"/>
       <c r="T57" s="7"/>
-      <c r="U57" s="7"/>
+      <c r="U57" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="V57" s="7"/>
       <c r="W57" s="7"/>
       <c r="X57" s="7"/>
       <c r="Y57" s="7"/>
       <c r="Z57" s="8" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="AA57" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB57" s="7"/>
+        <v>42</v>
+      </c>
+      <c r="AB57" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="58" spans="1:28">
       <c r="A58" s="3">
         <v>56</v>
       </c>
       <c r="B58" s="3">
-        <v>2025100067</v>
+        <v>2025100516</v>
       </c>
       <c r="C58" s="3">
         <v>1</v>
@@ -5002,42 +5085,42 @@
         <v>122</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>44</v>
+        <v>196</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="I58" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="J58" s="3" t="s">
         <v>198</v>
-      </c>
-      <c r="J58" s="3" t="s">
-        <v>188</v>
       </c>
       <c r="K58" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L58" s="6" t="s">
-        <v>150</v>
+        <v>199</v>
       </c>
       <c r="M58" s="6" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="N58" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="O58" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P58" s="3"/>
       <c r="Q58" s="3"/>
       <c r="R58" s="3">
-        <v>942</v>
+        <v>297956</v>
       </c>
       <c r="S58" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T58" s="3"/>
       <c r="U58" s="3"/>
@@ -5046,21 +5129,17 @@
       <c r="X58" s="3"/>
       <c r="Y58" s="3"/>
       <c r="Z58" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA58" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB58" s="3">
-        <v>1</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="AA58" s="3"/>
+      <c r="AB58" s="3"/>
     </row>
     <row r="59" spans="1:28">
       <c r="A59" s="7">
         <v>57</v>
       </c>
       <c r="B59" s="7">
-        <v>2025100068</v>
+        <v>2025100517</v>
       </c>
       <c r="C59" s="7">
         <v>1</v>
@@ -5072,39 +5151,39 @@
         <v>122</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>44</v>
+        <v>196</v>
       </c>
       <c r="H59" s="7" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="I59" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="J59" s="7" t="s">
         <v>198</v>
-      </c>
-      <c r="J59" s="7" t="s">
-        <v>188</v>
       </c>
       <c r="K59" s="7" t="s">
         <v>36</v>
       </c>
       <c r="L59" s="8" t="s">
-        <v>150</v>
+        <v>199</v>
       </c>
       <c r="M59" s="8" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="N59" s="8" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="O59" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P59" s="7"/>
       <c r="Q59" s="7"/>
       <c r="R59" s="7">
-        <v>942</v>
+        <v>297956</v>
       </c>
       <c r="S59" s="7"/>
       <c r="T59" s="7"/>
@@ -5114,10 +5193,10 @@
       <c r="X59" s="7"/>
       <c r="Y59" s="7"/>
       <c r="Z59" s="8" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="AA59" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB59" s="7"/>
     </row>
@@ -5126,7 +5205,7 @@
         <v>58</v>
       </c>
       <c r="B60" s="3">
-        <v>2025100505</v>
+        <v>2025100511</v>
       </c>
       <c r="C60" s="3">
         <v>1</v>
@@ -5141,39 +5220,39 @@
         <v>85</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>143</v>
+        <v>87</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>144</v>
+        <v>196</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="K60" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L60" s="6" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="M60" s="6" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="N60" s="6" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="O60" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P60" s="3"/>
       <c r="Q60" s="3"/>
       <c r="R60" s="3">
-        <v>187561</v>
+        <v>117288</v>
       </c>
       <c r="S60" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T60" s="3"/>
       <c r="U60" s="3"/>
@@ -5182,7 +5261,7 @@
       <c r="X60" s="3"/>
       <c r="Y60" s="3"/>
       <c r="Z60" s="6" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="AA60" s="3"/>
       <c r="AB60" s="3"/>
@@ -5192,7 +5271,7 @@
         <v>59</v>
       </c>
       <c r="B61" s="7">
-        <v>2025100506</v>
+        <v>2025100512</v>
       </c>
       <c r="C61" s="7">
         <v>1</v>
@@ -5207,36 +5286,36 @@
         <v>85</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>143</v>
+        <v>87</v>
       </c>
       <c r="H61" s="7" t="s">
-        <v>144</v>
+        <v>196</v>
       </c>
       <c r="I61" s="7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="J61" s="7" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="K61" s="7" t="s">
         <v>36</v>
       </c>
       <c r="L61" s="8" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="M61" s="8" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="N61" s="8" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="O61" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P61" s="7"/>
       <c r="Q61" s="7"/>
       <c r="R61" s="7">
-        <v>187561</v>
+        <v>117288</v>
       </c>
       <c r="S61" s="7"/>
       <c r="T61" s="7"/>
@@ -5246,10 +5325,10 @@
       <c r="X61" s="7"/>
       <c r="Y61" s="7"/>
       <c r="Z61" s="8" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="AA61" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB61" s="7"/>
     </row>
@@ -5258,7 +5337,7 @@
         <v>60</v>
       </c>
       <c r="B62" s="3">
-        <v>2025100508</v>
+        <v>2025100072</v>
       </c>
       <c r="C62" s="3">
         <v>1</v>
@@ -5270,42 +5349,42 @@
         <v>122</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>144</v>
+        <v>97</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>87</v>
+        <v>155</v>
       </c>
       <c r="I62" s="3" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="K62" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L62" s="6" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="M62" s="6" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="N62" s="6" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="O62" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P62" s="3"/>
       <c r="Q62" s="3"/>
       <c r="R62" s="3">
-        <v>367919</v>
+        <v>54</v>
       </c>
       <c r="S62" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T62" s="3"/>
       <c r="U62" s="3"/>
@@ -5314,17 +5393,21 @@
       <c r="X62" s="3"/>
       <c r="Y62" s="3"/>
       <c r="Z62" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA62" s="3"/>
-      <c r="AB62" s="3"/>
+        <v>128</v>
+      </c>
+      <c r="AA62" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB62" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="63" spans="1:28">
       <c r="A63" s="7">
         <v>61</v>
       </c>
       <c r="B63" s="7">
-        <v>2025100509</v>
+        <v>2025100073</v>
       </c>
       <c r="C63" s="7">
         <v>1</v>
@@ -5336,39 +5419,39 @@
         <v>122</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
       <c r="G63" s="7" t="s">
-        <v>144</v>
+        <v>97</v>
       </c>
       <c r="H63" s="7" t="s">
-        <v>87</v>
+        <v>155</v>
       </c>
       <c r="I63" s="7" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="J63" s="7" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="K63" s="7" t="s">
         <v>36</v>
       </c>
       <c r="L63" s="8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="M63" s="8" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="N63" s="8" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="O63" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P63" s="7"/>
       <c r="Q63" s="7"/>
       <c r="R63" s="7">
-        <v>367919</v>
+        <v>54</v>
       </c>
       <c r="S63" s="7"/>
       <c r="T63" s="7"/>
@@ -5378,10 +5461,10 @@
       <c r="X63" s="7"/>
       <c r="Y63" s="7"/>
       <c r="Z63" s="8" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="AA63" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB63" s="7"/>
     </row>
@@ -5390,7 +5473,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="3">
-        <v>2025100079</v>
+        <v>2025100067</v>
       </c>
       <c r="C64" s="3">
         <v>1</v>
@@ -5405,39 +5488,39 @@
         <v>31</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>136</v>
+        <v>44</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>143</v>
+        <v>96</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="J64" s="3" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="K64" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L64" s="6" t="s">
-        <v>138</v>
+        <v>157</v>
       </c>
       <c r="M64" s="6" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="N64" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="O64" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P64" s="3"/>
       <c r="Q64" s="3"/>
       <c r="R64" s="3">
-        <v>68795</v>
+        <v>942</v>
       </c>
       <c r="S64" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T64" s="3"/>
       <c r="U64" s="3"/>
@@ -5446,17 +5529,21 @@
       <c r="X64" s="3"/>
       <c r="Y64" s="3"/>
       <c r="Z64" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA64" s="3"/>
-      <c r="AB64" s="3"/>
+        <v>128</v>
+      </c>
+      <c r="AA64" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB64" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="65" spans="1:28">
       <c r="A65" s="7">
         <v>63</v>
       </c>
       <c r="B65" s="7">
-        <v>2025100080</v>
+        <v>2025100068</v>
       </c>
       <c r="C65" s="7">
         <v>1</v>
@@ -5471,36 +5558,36 @@
         <v>31</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>136</v>
+        <v>44</v>
       </c>
       <c r="H65" s="7" t="s">
-        <v>143</v>
+        <v>96</v>
       </c>
       <c r="I65" s="7" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="J65" s="7" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="K65" s="7" t="s">
         <v>36</v>
       </c>
       <c r="L65" s="8" t="s">
-        <v>138</v>
+        <v>157</v>
       </c>
       <c r="M65" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="N65" s="8" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="O65" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P65" s="7"/>
       <c r="Q65" s="7"/>
       <c r="R65" s="7">
-        <v>68795</v>
+        <v>942</v>
       </c>
       <c r="S65" s="7"/>
       <c r="T65" s="7"/>
@@ -5510,10 +5597,10 @@
       <c r="X65" s="7"/>
       <c r="Y65" s="7"/>
       <c r="Z65" s="8" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="AA65" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB65" s="7"/>
     </row>
@@ -5522,7 +5609,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="3">
-        <v>2025100009</v>
+        <v>2025100505</v>
       </c>
       <c r="C66" s="3">
         <v>1</v>
@@ -5534,41 +5621,43 @@
         <v>122</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>97</v>
+        <v>151</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>120</v>
+        <v>152</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="J66" s="3" t="s">
-        <v>78</v>
+        <v>198</v>
       </c>
       <c r="K66" s="3" t="s">
-        <v>79</v>
+        <v>36</v>
       </c>
       <c r="L66" s="6" t="s">
-        <v>80</v>
+        <v>171</v>
       </c>
       <c r="M66" s="6" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="N66" s="6" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="O66" s="3" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="P66" s="3"/>
       <c r="Q66" s="3"/>
       <c r="R66" s="3">
-        <v>0</v>
-      </c>
-      <c r="S66" s="3"/>
+        <v>187561</v>
+      </c>
+      <c r="S66" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="T66" s="3"/>
       <c r="U66" s="3"/>
       <c r="V66" s="3"/>
@@ -5576,21 +5665,17 @@
       <c r="X66" s="3"/>
       <c r="Y66" s="3"/>
       <c r="Z66" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="AA66" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB66" s="3">
-        <v>1</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="AA66" s="3"/>
+      <c r="AB66" s="3"/>
     </row>
     <row r="67" spans="1:28">
       <c r="A67" s="7">
         <v>65</v>
       </c>
       <c r="B67" s="7">
-        <v>2025100042</v>
+        <v>2025100506</v>
       </c>
       <c r="C67" s="7">
         <v>1</v>
@@ -5602,27 +5687,31 @@
         <v>122</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>120</v>
+        <v>151</v>
       </c>
       <c r="H67" s="7" t="s">
-        <v>214</v>
+        <v>152</v>
       </c>
       <c r="I67" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="J67" s="7"/>
-      <c r="K67" s="7"/>
+        <v>211</v>
+      </c>
+      <c r="J67" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="K67" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="L67" s="8" t="s">
-        <v>80</v>
+        <v>171</v>
       </c>
       <c r="M67" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="N67" s="8" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="O67" s="7" t="s">
         <v>40</v>
@@ -5630,11 +5719,9 @@
       <c r="P67" s="7"/>
       <c r="Q67" s="7"/>
       <c r="R67" s="7">
-        <v>0</v>
-      </c>
-      <c r="S67" s="7" t="s">
-        <v>41</v>
-      </c>
+        <v>187561</v>
+      </c>
+      <c r="S67" s="7"/>
       <c r="T67" s="7"/>
       <c r="U67" s="7"/>
       <c r="V67" s="7"/>
@@ -5642,45 +5729,781 @@
       <c r="X67" s="7"/>
       <c r="Y67" s="7"/>
       <c r="Z67" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="AA67" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB67" s="7"/>
+    </row>
+    <row r="68" spans="1:28">
+      <c r="A68" s="3">
+        <v>66</v>
+      </c>
+      <c r="B68" s="3">
+        <v>2025100508</v>
+      </c>
+      <c r="C68" s="3">
+        <v>1</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="H68" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I68" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="J68" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="K68" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L68" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="M68" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="N68" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="O68" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="P68" s="3"/>
+      <c r="Q68" s="3"/>
+      <c r="R68" s="3">
+        <v>367919</v>
+      </c>
+      <c r="S68" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="T68" s="3"/>
+      <c r="U68" s="3"/>
+      <c r="V68" s="3"/>
+      <c r="W68" s="3"/>
+      <c r="X68" s="3"/>
+      <c r="Y68" s="3"/>
+      <c r="Z68" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="AA68" s="3"/>
+      <c r="AB68" s="3"/>
+    </row>
+    <row r="69" spans="1:28">
+      <c r="A69" s="7">
+        <v>67</v>
+      </c>
+      <c r="B69" s="7">
+        <v>2025100509</v>
+      </c>
+      <c r="C69" s="7">
+        <v>1</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E69" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G69" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="H69" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I69" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="J69" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="K69" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="L69" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="M69" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="N69" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="O69" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="P69" s="7"/>
+      <c r="Q69" s="7"/>
+      <c r="R69" s="7">
+        <v>367919</v>
+      </c>
+      <c r="S69" s="7"/>
+      <c r="T69" s="7"/>
+      <c r="U69" s="7"/>
+      <c r="V69" s="7"/>
+      <c r="W69" s="7"/>
+      <c r="X69" s="7"/>
+      <c r="Y69" s="7"/>
+      <c r="Z69" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="AA69" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB69" s="7"/>
+    </row>
+    <row r="70" spans="1:28">
+      <c r="A70" s="3">
+        <v>68</v>
+      </c>
+      <c r="B70" s="3">
+        <v>2025100559</v>
+      </c>
+      <c r="C70" s="3">
+        <v>1</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="H70" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="I70" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="J70" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="K70" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L70" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="M70" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="N70" s="6"/>
+      <c r="O70" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="P70" s="3"/>
+      <c r="Q70" s="3"/>
+      <c r="R70" s="3">
+        <v>140018</v>
+      </c>
+      <c r="S70" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="T70" s="3"/>
+      <c r="U70" s="3"/>
+      <c r="V70" s="3"/>
+      <c r="W70" s="3"/>
+      <c r="X70" s="3"/>
+      <c r="Y70" s="3"/>
+      <c r="Z70" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="AA70" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB70" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:28">
+      <c r="A71" s="7">
+        <v>69</v>
+      </c>
+      <c r="B71" s="7">
+        <v>2025100560</v>
+      </c>
+      <c r="C71" s="7">
+        <v>1</v>
+      </c>
+      <c r="D71" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F71" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="G71" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="H71" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="I71" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="J71" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="K71" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="L71" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="M71" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="N71" s="8"/>
+      <c r="O71" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="P71" s="7"/>
+      <c r="Q71" s="7"/>
+      <c r="R71" s="7">
+        <v>140018</v>
+      </c>
+      <c r="S71" s="7"/>
+      <c r="T71" s="7"/>
+      <c r="U71" s="7"/>
+      <c r="V71" s="7"/>
+      <c r="W71" s="7"/>
+      <c r="X71" s="7"/>
+      <c r="Y71" s="7"/>
+      <c r="Z71" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="AA71" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB71" s="7"/>
+    </row>
+    <row r="72" spans="1:28">
+      <c r="A72" s="3">
+        <v>70</v>
+      </c>
+      <c r="B72" s="3">
+        <v>2025100557</v>
+      </c>
+      <c r="C72" s="3">
+        <v>1</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="H72" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I72" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="J72" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="K72" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L72" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="M72" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="N72" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="O72" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="P72" s="3"/>
+      <c r="Q72" s="3">
+        <v>3480</v>
+      </c>
+      <c r="R72" s="3">
+        <v>8923</v>
+      </c>
+      <c r="S72" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="T72" s="3"/>
+      <c r="U72" s="3"/>
+      <c r="V72" s="3"/>
+      <c r="W72" s="3"/>
+      <c r="X72" s="3"/>
+      <c r="Y72" s="3"/>
+      <c r="Z72" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="AA72" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB72" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:28">
+      <c r="A73" s="7">
+        <v>71</v>
+      </c>
+      <c r="B73" s="7">
+        <v>2025100558</v>
+      </c>
+      <c r="C73" s="7">
+        <v>1</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F73" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="G73" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="H73" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="I73" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="J73" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="K73" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="L73" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="M73" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="N73" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="O73" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="P73" s="7"/>
+      <c r="Q73" s="7">
+        <v>3480</v>
+      </c>
+      <c r="R73" s="7">
+        <v>8923</v>
+      </c>
+      <c r="S73" s="7"/>
+      <c r="T73" s="7"/>
+      <c r="U73" s="7"/>
+      <c r="V73" s="7"/>
+      <c r="W73" s="7"/>
+      <c r="X73" s="7"/>
+      <c r="Y73" s="7"/>
+      <c r="Z73" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="AA73" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB73" s="7"/>
+    </row>
+    <row r="74" spans="1:28">
+      <c r="A74" s="3">
+        <v>72</v>
+      </c>
+      <c r="B74" s="3">
+        <v>2025100079</v>
+      </c>
+      <c r="C74" s="3">
+        <v>1</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="H74" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="I74" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="J74" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="K74" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L74" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="M74" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="N74" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="O74" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="P74" s="3"/>
+      <c r="Q74" s="3"/>
+      <c r="R74" s="3">
+        <v>68795</v>
+      </c>
+      <c r="S74" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="T74" s="3"/>
+      <c r="U74" s="3"/>
+      <c r="V74" s="3"/>
+      <c r="W74" s="3"/>
+      <c r="X74" s="3"/>
+      <c r="Y74" s="3"/>
+      <c r="Z74" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="AA74" s="3"/>
+      <c r="AB74" s="3"/>
+    </row>
+    <row r="75" spans="1:28">
+      <c r="A75" s="7">
+        <v>73</v>
+      </c>
+      <c r="B75" s="7">
+        <v>2025100080</v>
+      </c>
+      <c r="C75" s="7">
+        <v>1</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E75" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F75" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G75" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="H75" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="I75" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="J75" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="K75" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="L75" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="M75" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="N75" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="O75" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="P75" s="7"/>
+      <c r="Q75" s="7"/>
+      <c r="R75" s="7">
+        <v>68795</v>
+      </c>
+      <c r="S75" s="7"/>
+      <c r="T75" s="7"/>
+      <c r="U75" s="7"/>
+      <c r="V75" s="7"/>
+      <c r="W75" s="7"/>
+      <c r="X75" s="7"/>
+      <c r="Y75" s="7"/>
+      <c r="Z75" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="AA75" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB75" s="7"/>
+    </row>
+    <row r="76" spans="1:28">
+      <c r="A76" s="3">
+        <v>74</v>
+      </c>
+      <c r="B76" s="3">
+        <v>2025100009</v>
+      </c>
+      <c r="C76" s="3">
+        <v>1</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H76" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I76" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="J76" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="K76" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L76" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="M76" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="N76" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="O76" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="P76" s="3"/>
+      <c r="Q76" s="3"/>
+      <c r="R76" s="3">
+        <v>0</v>
+      </c>
+      <c r="S76" s="3"/>
+      <c r="T76" s="3"/>
+      <c r="U76" s="3"/>
+      <c r="V76" s="3"/>
+      <c r="W76" s="3"/>
+      <c r="X76" s="3"/>
+      <c r="Y76" s="3"/>
+      <c r="Z76" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="AA76" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB76" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:28">
+      <c r="A77" s="7">
+        <v>75</v>
+      </c>
+      <c r="B77" s="7">
+        <v>2025100042</v>
+      </c>
+      <c r="C77" s="7">
+        <v>1</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E77" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F77" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G77" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="H77" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="I77" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="J77" s="7"/>
+      <c r="K77" s="7"/>
+      <c r="L77" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="M77" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="N77" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="O77" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="P77" s="7"/>
+      <c r="Q77" s="7"/>
+      <c r="R77" s="7">
+        <v>0</v>
+      </c>
+      <c r="S77" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="T77" s="7"/>
+      <c r="U77" s="7"/>
+      <c r="V77" s="7"/>
+      <c r="W77" s="7"/>
+      <c r="X77" s="7"/>
+      <c r="Y77" s="7"/>
+      <c r="Z77" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="AA67" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB67" s="7"/>
-    </row>
-    <row r="68" spans="1:28">
-      <c r="A68" s="9"/>
-      <c r="B68" s="9"/>
-      <c r="C68" s="9"/>
-      <c r="D68" s="9"/>
-      <c r="E68" s="9"/>
-      <c r="F68" s="9"/>
-      <c r="G68" s="9"/>
-      <c r="H68" s="9"/>
-      <c r="I68" s="9"/>
-      <c r="J68" s="9"/>
-      <c r="K68" s="9"/>
-      <c r="L68" s="10"/>
-      <c r="M68" s="10"/>
-      <c r="N68" s="10"/>
-      <c r="O68" s="9"/>
-      <c r="P68" s="9"/>
-      <c r="Q68" s="9"/>
-      <c r="R68" s="9"/>
-      <c r="S68" s="9"/>
-      <c r="T68" s="9"/>
-      <c r="U68" s="9"/>
-      <c r="V68" s="9"/>
-      <c r="W68" s="9"/>
-      <c r="X68" s="9"/>
-      <c r="Y68" s="9"/>
-      <c r="Z68" s="10"/>
-      <c r="AA68" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="AB68" s="9">
-        <v>30</v>
+      <c r="AA77" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB77" s="7"/>
+    </row>
+    <row r="78" spans="1:28">
+      <c r="A78" s="3">
+        <v>76</v>
+      </c>
+      <c r="B78" s="3">
+        <v>2025100636</v>
+      </c>
+      <c r="C78" s="3">
+        <v>1</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H78" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="I78" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="J78" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="K78" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="L78" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="M78" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="N78" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="O78" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="P78" s="3"/>
+      <c r="Q78" s="3"/>
+      <c r="R78" s="3">
+        <v>0</v>
+      </c>
+      <c r="S78" s="3"/>
+      <c r="T78" s="3"/>
+      <c r="U78" s="3"/>
+      <c r="V78" s="3"/>
+      <c r="W78" s="3"/>
+      <c r="X78" s="3"/>
+      <c r="Y78" s="3"/>
+      <c r="Z78" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="AA78" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB78" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:28">
+      <c r="A79" s="9"/>
+      <c r="B79" s="9"/>
+      <c r="C79" s="9"/>
+      <c r="D79" s="9"/>
+      <c r="E79" s="9"/>
+      <c r="F79" s="9"/>
+      <c r="G79" s="9"/>
+      <c r="H79" s="9"/>
+      <c r="I79" s="9"/>
+      <c r="J79" s="9"/>
+      <c r="K79" s="9"/>
+      <c r="L79" s="10"/>
+      <c r="M79" s="10"/>
+      <c r="N79" s="10"/>
+      <c r="O79" s="9"/>
+      <c r="P79" s="9"/>
+      <c r="Q79" s="9"/>
+      <c r="R79" s="9"/>
+      <c r="S79" s="9"/>
+      <c r="T79" s="9"/>
+      <c r="U79" s="9"/>
+      <c r="V79" s="9"/>
+      <c r="W79" s="9"/>
+      <c r="X79" s="9"/>
+      <c r="Y79" s="9"/>
+      <c r="Z79" s="10"/>
+      <c r="AA79" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="AB79" s="9">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>